<commit_message>
Looking very good now. Squashed a bug when transfering asset value from company to private
</commit_message>
<xml_diff>
--- a/tests/Feature/config/company-private-transfer_tenpercent.xlsx
+++ b/tests/Feature/config/company-private-transfer_tenpercent.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="101">
   <si>
     <t>Sum total</t>
   </si>
@@ -181,9 +181,6 @@
     <t xml:space="preserve"> Company dividend tax on originalAmount: 1361998, originalTaxAmount: 102102, dividendTaxAmount:514835, newTaxAmount: 616937, realizationamount: 847163</t>
   </si>
   <si>
-    <t xml:space="preserve"> Company dividend tax on originalAmount: 7964.2, originalTaxAmount: 104348, dividendTaxAmount:3010, newTaxAmount: 107358, realizationamount: 4954</t>
-  </si>
-  <si>
     <t>Fond - Firma</t>
   </si>
   <si>
@@ -203,9 +200,6 @@
   </si>
   <si>
     <t xml:space="preserve"> Asset rule: Using current amount: 1331000 * 1 </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Asset rule:100% 100% of 1464100=1464100</t>
   </si>
   <si>
     <t>Fond - Privat</t>
@@ -2342,13 +2336,13 @@
       </c>
       <c r="O20" s="2"/>
       <c r="P20" s="6">
-        <v>1092930.0316</v>
+        <v>980618.0</v>
       </c>
       <c r="Q20" s="2">
-        <v>0.32</v>
+        <v>0.39</v>
       </c>
       <c r="R20" s="1">
-        <v>1092930.0316</v>
+        <v>980618.0</v>
       </c>
       <c r="S20" s="1">
         <v>845060.756</v>
@@ -2357,11 +2351,11 @@
         <v>845060.756</v>
       </c>
       <c r="U20" s="1">
-        <v>1739350.8</v>
+        <v>128840.8</v>
       </c>
       <c r="V20" s="2"/>
       <c r="W20" s="5">
-        <v>393.508</v>
+        <v>0.0</v>
       </c>
       <c r="X20" s="2"/>
       <c r="Y20" s="5">
@@ -2369,13 +2363,13 @@
       </c>
       <c r="Z20" s="2"/>
       <c r="AA20" s="1">
-        <v>937287.0316</v>
+        <v>929323.0</v>
       </c>
       <c r="AB20" s="1">
-        <v>609867.2756</v>
+        <v>135557.244</v>
       </c>
       <c r="AC20" s="5">
-        <v>155643.0</v>
+        <v>51295.0</v>
       </c>
       <c r="AD20" s="2"/>
       <c r="AE20" s="1">
@@ -2442,7 +2436,7 @@
         <v>1078680.0</v>
       </c>
       <c r="Q21" s="2">
-        <v>0.01</v>
+        <v>0.1</v>
       </c>
       <c r="R21" s="1">
         <v>1078680.0</v>
@@ -8298,13 +8292,13 @@
       </c>
       <c r="O20" s="2"/>
       <c r="P20" s="6">
-        <v>980617.8316</v>
+        <v>980618.0</v>
       </c>
       <c r="Q20" s="2">
         <v>5.69</v>
       </c>
       <c r="R20" s="1">
-        <v>980617.8316</v>
+        <v>980618.0</v>
       </c>
       <c r="S20" s="1">
         <v>845060.756</v>
@@ -8325,10 +8319,10 @@
       </c>
       <c r="Z20" s="2"/>
       <c r="AA20" s="1">
-        <v>929322.8316</v>
+        <v>929323.0</v>
       </c>
       <c r="AB20" s="1">
-        <v>135557.0756</v>
+        <v>135557.244</v>
       </c>
       <c r="AC20" s="5">
         <v>51295.0</v>
@@ -14272,13 +14266,11 @@
       </c>
       <c r="O20" s="2"/>
       <c r="P20" s="6">
-        <v>112312.2</v>
-      </c>
-      <c r="Q20" s="2">
-        <v>0.92</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="Q20" s="2"/>
       <c r="R20" s="1">
-        <v>112312.2</v>
+        <v>0</v>
       </c>
       <c r="S20" s="1">
         <v>0</v>
@@ -14287,11 +14279,11 @@
         <v>0</v>
       </c>
       <c r="U20" s="1">
-        <v>1610510</v>
+        <v>0</v>
       </c>
       <c r="V20" s="2"/>
       <c r="W20" s="5">
-        <v>16105.1</v>
+        <v>0.0</v>
       </c>
       <c r="X20" s="2"/>
       <c r="Y20" s="5">
@@ -14299,17 +14291,15 @@
       </c>
       <c r="Z20" s="2"/>
       <c r="AA20" s="1">
-        <v>4954.0</v>
+        <v>0</v>
       </c>
       <c r="AB20" s="1">
-        <v>474310.2</v>
+        <v>0</v>
       </c>
       <c r="AC20" s="5">
-        <v>107358.0</v>
-      </c>
-      <c r="AD20" s="2">
-        <v>0.378</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="AD20" s="2"/>
       <c r="AE20" s="1">
         <v>0</v>
       </c>
@@ -14332,9 +14322,7 @@
       </c>
       <c r="AM20" s="1"/>
       <c r="AN20" s="2"/>
-      <c r="AO20" t="s">
-        <v>53</v>
-      </c>
+      <c r="AO20"/>
     </row>
     <row r="21" spans="1:41">
       <c r="A21">
@@ -18599,7 +18587,7 @@
   <sheetData>
     <row r="1" spans="1:41">
       <c r="A1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:41">
@@ -18607,19 +18595,19 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E2" t="s">
         <v>3</v>
       </c>
       <c r="F2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G2" t="s">
         <v>4</v>
@@ -18631,7 +18619,7 @@
         <v>5</v>
       </c>
       <c r="J2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:41">
@@ -19412,7 +19400,7 @@
         <v>1</v>
       </c>
       <c r="AO15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:41">
@@ -19499,7 +19487,7 @@
       <c r="AM16" s="1"/>
       <c r="AN16" s="2"/>
       <c r="AO16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="17" spans="1:41">
@@ -19586,7 +19574,7 @@
       <c r="AM17" s="1"/>
       <c r="AN17" s="2"/>
       <c r="AO17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="18" spans="1:41">
@@ -19673,7 +19661,7 @@
       <c r="AM18" s="1"/>
       <c r="AN18" s="2"/>
       <c r="AO18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="19" spans="1:41">
@@ -19760,7 +19748,7 @@
       <c r="AM19" s="8"/>
       <c r="AN19" s="9"/>
       <c r="AO19" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="20" spans="1:41">
@@ -19785,48 +19773,22 @@
       <c r="M20" s="1"/>
       <c r="N20" s="1"/>
       <c r="O20" s="2"/>
-      <c r="P20" s="6">
-        <v>112312.2</v>
-      </c>
-      <c r="Q20" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="R20" s="1">
-        <v>112312.2</v>
-      </c>
-      <c r="S20" s="1">
-        <v>0</v>
-      </c>
-      <c r="T20" s="1">
-        <v>0</v>
-      </c>
-      <c r="U20" s="1">
-        <v>1610510</v>
-      </c>
-      <c r="V20" s="2">
-        <v>1</v>
-      </c>
-      <c r="W20" s="5">
-        <v>0</v>
-      </c>
+      <c r="P20" s="6"/>
+      <c r="Q20" s="2"/>
+      <c r="R20" s="1"/>
+      <c r="S20" s="1"/>
+      <c r="T20" s="1"/>
+      <c r="U20" s="1"/>
+      <c r="V20" s="2"/>
+      <c r="W20" s="5"/>
       <c r="X20" s="2"/>
       <c r="Y20" s="5"/>
       <c r="Z20" s="2"/>
-      <c r="AA20" s="1">
-        <v>7964.2</v>
-      </c>
-      <c r="AB20" s="1">
-        <v>474310.2</v>
-      </c>
-      <c r="AC20" s="5">
-        <v>104348.0</v>
-      </c>
-      <c r="AD20" s="2">
-        <v>0.22</v>
-      </c>
-      <c r="AE20" s="1">
-        <v>0.0</v>
-      </c>
+      <c r="AA20" s="1"/>
+      <c r="AB20" s="1"/>
+      <c r="AC20" s="5"/>
+      <c r="AD20" s="2"/>
+      <c r="AE20" s="1"/>
       <c r="AF20" s="2"/>
       <c r="AG20" s="6">
         <v>0.0</v>
@@ -19846,9 +19808,7 @@
       </c>
       <c r="AM20" s="1"/>
       <c r="AN20" s="2"/>
-      <c r="AO20" t="s">
-        <v>61</v>
-      </c>
+      <c r="AO20"/>
     </row>
     <row r="21" spans="1:41">
       <c r="A21">
@@ -22961,7 +22921,7 @@
   <sheetData>
     <row r="1" spans="1:41">
       <c r="A1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:41">
@@ -22969,19 +22929,19 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E2" t="s">
         <v>3</v>
       </c>
       <c r="F2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G2" t="s">
         <v>4</v>
@@ -22993,7 +22953,7 @@
         <v>5</v>
       </c>
       <c r="J2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:41">
@@ -23774,7 +23734,7 @@
         <v>1</v>
       </c>
       <c r="AO15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="16" spans="1:41">
@@ -23861,7 +23821,7 @@
       <c r="AM16" s="1"/>
       <c r="AN16" s="2"/>
       <c r="AO16" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="17" spans="1:41">
@@ -23948,7 +23908,7 @@
       <c r="AM17" s="1"/>
       <c r="AN17" s="2"/>
       <c r="AO17" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="18" spans="1:41">
@@ -24035,7 +23995,7 @@
       <c r="AM18" s="1"/>
       <c r="AN18" s="2"/>
       <c r="AO18" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="19" spans="1:41">
@@ -24122,7 +24082,7 @@
       <c r="AM19" s="8"/>
       <c r="AN19" s="9"/>
       <c r="AO19" s="7" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="20" spans="1:41">
@@ -24148,13 +24108,13 @@
       <c r="N20" s="1"/>
       <c r="O20" s="2"/>
       <c r="P20" s="6">
-        <v>980617.8316</v>
+        <v>980618.0</v>
       </c>
       <c r="Q20" s="2">
         <v>0.1</v>
       </c>
       <c r="R20" s="1">
-        <v>980617.8316</v>
+        <v>980618.0</v>
       </c>
       <c r="S20" s="1">
         <v>845060.756</v>
@@ -24175,10 +24135,10 @@
       <c r="Y20" s="5"/>
       <c r="Z20" s="2"/>
       <c r="AA20" s="1">
-        <v>929322.8316</v>
+        <v>929323.0</v>
       </c>
       <c r="AB20" s="1">
-        <v>135557.0756</v>
+        <v>135557.244</v>
       </c>
       <c r="AC20" s="5">
         <v>51295.0</v>
@@ -24211,7 +24171,7 @@
         <v>1</v>
       </c>
       <c r="AO20" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="21" spans="1:41">
@@ -24298,7 +24258,7 @@
       <c r="AM21" s="1"/>
       <c r="AN21" s="2"/>
       <c r="AO21" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="22" spans="1:41">
@@ -24385,7 +24345,7 @@
       <c r="AM22" s="1"/>
       <c r="AN22" s="2"/>
       <c r="AO22" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="23" spans="1:41">
@@ -24472,7 +24432,7 @@
       <c r="AM23" s="1"/>
       <c r="AN23" s="2"/>
       <c r="AO23" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="24" spans="1:41">
@@ -24559,7 +24519,7 @@
       <c r="AM24" s="1"/>
       <c r="AN24" s="2"/>
       <c r="AO24" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="25" spans="1:41">
@@ -24646,7 +24606,7 @@
       <c r="AM25" s="1"/>
       <c r="AN25" s="2"/>
       <c r="AO25" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="26" spans="1:41">
@@ -24733,7 +24693,7 @@
       <c r="AM26" s="1"/>
       <c r="AN26" s="2"/>
       <c r="AO26" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="27" spans="1:41">
@@ -24820,7 +24780,7 @@
       <c r="AM27" s="1"/>
       <c r="AN27" s="2"/>
       <c r="AO27" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="28" spans="1:41">
@@ -24907,7 +24867,7 @@
       <c r="AM28" s="1"/>
       <c r="AN28" s="2"/>
       <c r="AO28" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="29" spans="1:41">
@@ -24996,7 +24956,7 @@
       <c r="AM29" s="1"/>
       <c r="AN29" s="2"/>
       <c r="AO29" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="30" spans="1:41">
@@ -25085,7 +25045,7 @@
       <c r="AM30" s="1"/>
       <c r="AN30" s="2"/>
       <c r="AO30" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="31" spans="1:41">
@@ -25174,7 +25134,7 @@
       <c r="AM31" s="1"/>
       <c r="AN31" s="2"/>
       <c r="AO31" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="32" spans="1:41">
@@ -25263,7 +25223,7 @@
       <c r="AM32" s="1"/>
       <c r="AN32" s="2"/>
       <c r="AO32" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="33" spans="1:41">
@@ -25352,7 +25312,7 @@
       <c r="AM33" s="1"/>
       <c r="AN33" s="2"/>
       <c r="AO33" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="34" spans="1:41">
@@ -25441,7 +25401,7 @@
       <c r="AM34" s="1"/>
       <c r="AN34" s="2"/>
       <c r="AO34" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="35" spans="1:41">
@@ -25530,7 +25490,7 @@
       <c r="AM35" s="1"/>
       <c r="AN35" s="2"/>
       <c r="AO35" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="36" spans="1:41">
@@ -25619,7 +25579,7 @@
       <c r="AM36" s="1"/>
       <c r="AN36" s="2"/>
       <c r="AO36" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="37" spans="1:41">
@@ -25708,7 +25668,7 @@
       <c r="AM37" s="1"/>
       <c r="AN37" s="2"/>
       <c r="AO37" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="38" spans="1:41">
@@ -25797,7 +25757,7 @@
       <c r="AM38" s="1"/>
       <c r="AN38" s="2"/>
       <c r="AO38" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="39" spans="1:41">
@@ -25886,7 +25846,7 @@
       <c r="AM39" s="1"/>
       <c r="AN39" s="2"/>
       <c r="AO39" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="40" spans="1:41">
@@ -25975,7 +25935,7 @@
       <c r="AM40" s="11"/>
       <c r="AN40" s="12"/>
       <c r="AO40" s="10" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="41" spans="1:41">
@@ -26064,7 +26024,7 @@
       <c r="AM41" s="1"/>
       <c r="AN41" s="2"/>
       <c r="AO41" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="42" spans="1:41">
@@ -26153,7 +26113,7 @@
       <c r="AM42" s="1"/>
       <c r="AN42" s="2"/>
       <c r="AO42" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="43" spans="1:41">
@@ -26242,7 +26202,7 @@
       <c r="AM43" s="1"/>
       <c r="AN43" s="2"/>
       <c r="AO43" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="44" spans="1:41">
@@ -26331,7 +26291,7 @@
       <c r="AM44" s="1"/>
       <c r="AN44" s="2"/>
       <c r="AO44" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="45" spans="1:41">
@@ -26420,7 +26380,7 @@
       <c r="AM45" s="1"/>
       <c r="AN45" s="2"/>
       <c r="AO45" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="46" spans="1:41">
@@ -26509,7 +26469,7 @@
       <c r="AM46" s="1"/>
       <c r="AN46" s="2"/>
       <c r="AO46" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="47" spans="1:41">
@@ -26598,7 +26558,7 @@
       <c r="AM47" s="1"/>
       <c r="AN47" s="2"/>
       <c r="AO47" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="48" spans="1:41">
@@ -26687,7 +26647,7 @@
       <c r="AM48" s="1"/>
       <c r="AN48" s="2"/>
       <c r="AO48" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="49" spans="1:41">
@@ -26776,7 +26736,7 @@
       <c r="AM49" s="1"/>
       <c r="AN49" s="2"/>
       <c r="AO49" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="50" spans="1:41">
@@ -26865,7 +26825,7 @@
       <c r="AM50" s="1"/>
       <c r="AN50" s="2"/>
       <c r="AO50" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="51" spans="1:41">
@@ -26954,7 +26914,7 @@
       <c r="AM51" s="1"/>
       <c r="AN51" s="2"/>
       <c r="AO51" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="52" spans="1:41">
@@ -27043,7 +27003,7 @@
       <c r="AM52" s="5"/>
       <c r="AN52" s="16"/>
       <c r="AO52" s="15" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="53" spans="1:41">
@@ -28229,10 +28189,10 @@
   <sheetData>
     <row r="5" spans="1:3">
       <c r="B5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C5" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:3">

</xml_diff>